<commit_message>
Move render label to back
</commit_message>
<xml_diff>
--- a/!info/Российская газета.xlsx
+++ b/!info/Российская газета.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
     <t>Приволжье</t>
   </si>
@@ -52,12 +52,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -354,9 +361,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -368,24 +377,25 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>10531</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2">
-        <v>50000</v>
+        <f>B1</f>
+        <v>10531</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>30000</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
+        <v>50000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -393,8 +403,25 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <f>SUM(B1:B3)</f>
-        <v>90531</v>
+        <f>B3</f>
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <f>B5</f>
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>